<commit_message>
Extended unified config process to EAs and OPs
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/ExtendedAttributes.xlsx
+++ b/utils/config/ReferenceLists/ExtendedAttributes.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2023/EMStoSamples/CanadaTestConfiguration/ReferenceLists/BuildItUp/AsBuiltTraining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2F8EAB3-2BDB-4098-91EF-9EB43F22F7E5}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8C4999C-A9F4-475E-B888-05D8809D3C85}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="-16200" windowWidth="27630" windowHeight="15600" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
+    <workbookView xWindow="-28920" yWindow="-3030" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtendedAttributes" sheetId="1" r:id="rId1"/>
-    <sheet name="DropDownLists" sheetId="2" r:id="rId2"/>
+    <sheet name="DropdownLists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1547,24 +1547,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA14A41-9107-421E-8224-801D8144DA01}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2085,19 +2085,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F259C135-316D-4E6D-99E9-298DC78EB6DB}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
-    <col min="4" max="4" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" customWidth="1"/>
+    <col min="4" max="4" width="55.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>126</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>127</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>128</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>129</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>130</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>131</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>132</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>133</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>134</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>135</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>136</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>137</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>138</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>139</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>140</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>141</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>142</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>143</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>144</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>145</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>146</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>147</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>148</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>149</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
         <v>150</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>151</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>152</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>153</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
         <v>154</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>155</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>156</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
         <v>157</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
         <v>158</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
         <v>159</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" t="s">
         <v>160</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" t="s">
         <v>161</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" t="s">
         <v>162</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" t="s">
         <v>163</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" t="s">
         <v>164</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
         <v>165</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>166</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" t="s">
         <v>167</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>168</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" t="s">
         <v>169</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
         <v>170</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" t="s">
         <v>171</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" t="s">
         <v>172</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" t="s">
         <v>173</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>174</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C67" t="s">
         <v>175</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C68" t="s">
         <v>176</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>177</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>178</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
         <v>179</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>180</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>181</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>182</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
         <v>183</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
         <v>184</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>185</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
         <v>186</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
         <v>187</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C80" t="s">
         <v>188</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>189</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C82" t="s">
         <v>190</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C83" t="s">
         <v>191</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C84" t="s">
         <v>192</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
         <v>193</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
         <v>194</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C87" t="s">
         <v>195</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C88" t="s">
         <v>196</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C89" t="s">
         <v>197</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C90" t="s">
         <v>198</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
         <v>199</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
         <v>200</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C93" t="s">
         <v>201</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C94" t="s">
         <v>202</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
         <v>203</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C96" t="s">
         <v>204</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>205</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>206</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>207</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>208</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>209</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>210</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>211</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>212</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>213</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>214</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>215</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>216</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>217</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>218</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Updated Extended Attributes list
Added "Upload file name" because it exists in the Test environment
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/ExtendedAttributes.xlsx
+++ b/utils/config/ReferenceLists/ExtendedAttributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8C4999C-A9F4-475E-B888-05D8809D3C85}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C01BE9-67DE-463F-817C-3108A63D3211}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3030" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtendedAttributes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="224">
   <si>
     <t>id</t>
   </si>
@@ -684,6 +684,15 @@
   </si>
   <si>
     <t>The agency that conducted the sampling. The numbers at the start are the EMS agency ID.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Upload File Name</t>
+  </si>
+  <si>
+    <t>Used by EDT to tag observations by what upload file they came from.</t>
   </si>
 </sst>
 </file>
@@ -1545,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA14A41-9107-421E-8224-801D8144DA01}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2076,6 +2085,38 @@
         <v>80</v>
       </c>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>221</v>
+      </c>
+      <c r="F17" t="s">
+        <v>221</v>
+      </c>
+      <c r="G17" t="s">
+        <v>221</v>
+      </c>
+      <c r="H17" t="s">
+        <v>221</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2085,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F259C135-316D-4E6D-99E9-298DC78EB6DB}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>